<commit_message>
Code Moi Nhat 24/02/2024
</commit_message>
<xml_diff>
--- a/danhsachhopdong.xlsx
+++ b/danhsachhopdong.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Mã Hợp Đồng</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Tổng Tiền</t>
   </si>
   <si>
-    <t>Le</t>
+    <t>Đạt</t>
   </si>
   <si>
     <t>51H-063.25</t>
@@ -59,16 +59,22 @@
     <t>Lexus NX 350 F SPORT</t>
   </si>
   <si>
+    <t>51H-079.53</t>
+  </si>
+  <si>
+    <t>Honda CR-V</t>
+  </si>
+  <si>
+    <t>51H-101.01</t>
+  </si>
+  <si>
+    <t>Huyndai Solati</t>
+  </si>
+  <si>
     <t>51H-138.83</t>
   </si>
   <si>
     <t>Mercedes AMG G 63</t>
-  </si>
-  <si>
-    <t>51H-012.34</t>
-  </si>
-  <si>
-    <t>Kia K5 2.0 Luxury</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -165,13 +171,13 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>45344.0</v>
+        <v>45345.0</v>
       </c>
       <c r="F2" t="n">
+        <v>45345.0</v>
+      </c>
+      <c r="G2" t="n">
         <v>45347.0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>45351.0</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -180,7 +186,7 @@
         <v>1000000.0</v>
       </c>
       <c r="J2" t="n">
-        <v>4000000.0</v>
+        <v>2000000.0</v>
       </c>
     </row>
     <row r="3">
@@ -197,13 +203,13 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>45344.0</v>
+        <v>45345.0</v>
       </c>
       <c r="F3" t="n">
-        <v>45344.0</v>
+        <v>45345.0</v>
       </c>
       <c r="G3" t="n">
-        <v>45346.0</v>
+        <v>45347.0</v>
       </c>
       <c r="H3" t="n">
         <v>0.0</v>
@@ -229,22 +235,22 @@
         <v>16</v>
       </c>
       <c r="E4" t="n">
-        <v>45344.0</v>
+        <v>45345.0</v>
       </c>
       <c r="F4" t="n">
-        <v>45344.0</v>
+        <v>45345.0</v>
       </c>
       <c r="G4" t="n">
-        <v>45351.0</v>
+        <v>45347.0</v>
       </c>
       <c r="H4" t="n">
         <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>2000000.0</v>
+        <v>1100000.0</v>
       </c>
       <c r="J4" t="n">
-        <v>1.4E7</v>
+        <v>2200000.0</v>
       </c>
     </row>
     <row r="5">
@@ -261,13 +267,13 @@
         <v>18</v>
       </c>
       <c r="E5" t="n">
-        <v>45344.0</v>
+        <v>45345.0</v>
       </c>
       <c r="F5" t="n">
-        <v>45346.0</v>
+        <v>45345.0</v>
       </c>
       <c r="G5" t="n">
-        <v>45350.0</v>
+        <v>45347.0</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
@@ -276,7 +282,7 @@
         <v>1000000.0</v>
       </c>
       <c r="J5" t="n">
-        <v>4000000.0</v>
+        <v>2000000.0</v>
       </c>
     </row>
     <row r="6">
@@ -287,33 +293,33 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E6" t="n">
-        <v>45342.0</v>
+        <v>45345.0</v>
       </c>
       <c r="F6" t="n">
-        <v>45347.0</v>
+        <v>45345.0</v>
       </c>
       <c r="G6" t="n">
-        <v>45351.0</v>
+        <v>45349.0</v>
       </c>
       <c r="H6" t="n">
         <v>0.0</v>
       </c>
       <c r="I6" t="n">
-        <v>100000.0</v>
+        <v>2000000.0</v>
       </c>
       <c r="J6" t="n">
-        <v>400000.0</v>
+        <v>6000000.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -325,86 +331,22 @@
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>45345.0</v>
+        <v>45346.0</v>
       </c>
       <c r="F7" t="n">
-        <v>45347.0</v>
+        <v>45346.0</v>
       </c>
       <c r="G7" t="n">
-        <v>45351.0</v>
+        <v>45349.0</v>
       </c>
       <c r="H7" t="n">
         <v>0.0</v>
       </c>
       <c r="I7" t="n">
-        <v>10000.0</v>
+        <v>1000000.0</v>
       </c>
       <c r="J7" t="n">
-        <v>400000.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="n">
-        <v>45345.0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>45348.0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>45350.0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>600000.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="n">
-        <v>45342.0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>45347.0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>45351.0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>50000.0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>500000.0</v>
+        <v>4000000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>